<commit_message>
added captain america t shirt details
</commit_message>
<xml_diff>
--- a/Research/2018/March 2018/Products/Products_Mar2018.xlsx
+++ b/Research/2018/March 2018/Products/Products_Mar2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>S.No</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>B0182CXBFS</t>
+  </si>
+  <si>
+    <t>Captain America t shirt</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +562,7 @@
         <v>19</v>
       </c>
       <c r="C2">
-        <v>97</v>
+        <v>1.49</v>
       </c>
       <c r="D2">
         <v>5000</v>
@@ -590,6 +593,24 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
+      </c>
+      <c r="E3">
+        <v>280</v>
+      </c>
+      <c r="F3">
+        <v>3.91</v>
+      </c>
+      <c r="G3">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details related to cap america t shirt
</commit_message>
<xml_diff>
--- a/Research/2018/March 2018/Products/Products_Mar2018.xlsx
+++ b/Research/2018/March 2018/Products/Products_Mar2018.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
   <si>
     <t>S.No</t>
   </si>
@@ -277,6 +277,18 @@
   </si>
   <si>
     <t>PRV</t>
+  </si>
+  <si>
+    <t>Captain America T Shirt</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -691,7 +703,7 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,19 +1068,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1078,13 +1091,41 @@
       <c r="C1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
+      </c>
+      <c r="C2">
+        <v>78.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3">
+        <v>81.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>